<commit_message>
add more schema and information_schema cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/mysql_ddl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/mysql_ddl_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="196">
   <si>
     <t>TestID</t>
   </si>
@@ -544,10 +544,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>drop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>schema56</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -564,6 +560,166 @@
   </si>
   <si>
     <t>csv_containsAll</t>
+  </si>
+  <si>
+    <t>创建database,验证元数据信息保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建schema,验证元数据信息保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除database,验证元数据信息删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除schema,验证元数据信息删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_024</t>
+  </si>
+  <si>
+    <t>ddl_025</t>
+  </si>
+  <si>
+    <t>ddl_026</t>
+  </si>
+  <si>
+    <t>ddl_027</t>
+  </si>
+  <si>
+    <t>create database MYDDL_026;drop database MYDDL_026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create schema MYDDL_027;drop schema MYDDL_027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create database MYDDL_024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from information_schema.schemata where schema_name in ('META','DINGO','ROOT','MYSQL','INFORMATION_SCHEMA','MYDDL_024')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create schema MYDDL_025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from information_schema.schemata where schema_name in ('META','DINGO','ROOT','MYSQL','INFORMATION_SCHEMA','MYDDL_025')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from information_schema.schemata where schema_name in ('META','DINGO','ROOT','MYSQL','INFORMATION_SCHEMA','MYDDL_026')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_024.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_025.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_026.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_027.csv</t>
+  </si>
+  <si>
+    <t>select * from information_schema.schemata where schema_name in ('META','DINGO','ROOT','MYSQL','INFORMATION_SCHEMA','MYDDL_027')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义创建的schema中创建的表查看元数据信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information_Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义创建的schema中创建的表删除后查看元数据信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_028</t>
+  </si>
+  <si>
+    <t>ddl_029</t>
+  </si>
+  <si>
+    <t>create database MYDDL_028;create table MYDDL_028.MYDDL028_TBL01(id int, name varchar(20), primary key(id))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='MYDDL028_TBL01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_028.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_029.csv</t>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='MYDDL029_TBL01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create database MYDDL_029;create table MYDDL_029.MYDDL029_TBL01(id int, name varchar(20), primary key(id));drop table MYDDL_029.MYDDL029_TBL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MYSQL schema中创建的表查看元数据信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information_Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MYSQL schema中创建的表删除后查看元数据信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddl_030</t>
+  </si>
+  <si>
+    <t>ddl_031</t>
+  </si>
+  <si>
+    <t>create table MYSQL.MYDDL030_TBL01(id int not null auto_increment, name varchar(20), primary key(id))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table MYSQL.MYDDL031_TBL01(id int not null auto_increment, name varchar(20), primary key(id));drop table MYSQL.MYDDL031_TBL01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='MYDDL030_TBL01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='MYDDL031_TBL01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_030.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_031.csv</t>
   </si>
 </sst>
 </file>
@@ -938,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1712,23 +1868,271 @@
       <c r="D24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="I24" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="J24" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>152</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A27" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic type to upper case
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/mysql_ddl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/mysql_ddl_cases.xlsx
@@ -552,10 +552,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='$schema56' or `TABLE_SCHEMA` in ('MYSQL', 'INFORMATION_SCHEMA')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_023.csv</t>
   </si>
   <si>
@@ -720,6 +716,10 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/ddl/expectedresult/ddl_031.csv</t>
+  </si>
+  <si>
+    <t>select `TABLE_CATALOG`,`TABLE_SCHEMA`,`TABLE_NAME`,`TABLE_TYPE`,`ENGINE`,`VERSION`,`ROW_FORMAT`,`TABLE_ROWS`,`AVG_ROW_LENGTH`,`DATA_LENGTH`,`MAX_DATA_LENGTH`,`INDEX_LENGTH`,`DATA_FREE`,`AUTO_INCREMENT`,`UPDATE_TIME`,`CHECK_TIME`,`TABLE_COLLATION`,`CHECKSUM`,`CREATE_OPTIONS`,`TABLE_COMMENT` from information_schema.tables where `TABLE_NAME`='$schema56'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1869,7 +1869,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>147</v>
@@ -1878,24 +1878,24 @@
         <v>148</v>
       </c>
       <c r="I24" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>16</v>
@@ -1906,27 +1906,27 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="J25" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>16</v>
@@ -1937,27 +1937,27 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>16</v>
@@ -1968,27 +1968,27 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>16</v>
@@ -1999,140 +1999,140 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I29" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="J29" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="K29" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D32" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>